<commit_message>
new file in the feature branch
</commit_message>
<xml_diff>
--- a/git info.xlsx
+++ b/git info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBBDDE0-3E4B-42DD-A754-3182145258BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A5DA0B-4689-4742-97CA-1A971F93F926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="480" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>00 Введение в курс Git и GitHub 00</t>
   </si>
@@ -283,6 +283,24 @@
   </si>
   <si>
     <t>git cat-file -t/-p bfaf17c (sha1 hesh)</t>
+  </si>
+  <si>
+    <t>git branch &lt;branch name&gt;</t>
+  </si>
+  <si>
+    <t>git checkout -b &lt;branch name&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git branch </t>
+  </si>
+  <si>
+    <t>git branch -m &lt;new br name&gt;</t>
+  </si>
+  <si>
+    <t>git branch -d &lt;del branch name&gt;</t>
+  </si>
+  <si>
+    <t>git merge &lt;feature branch name&gt;</t>
   </si>
 </sst>
 </file>
@@ -1969,7 +1987,7 @@
   <dimension ref="B2:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2120,37 +2138,49 @@
       <c r="B19" s="2">
         <v>18</v>
       </c>
-      <c r="C19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>19</v>
       </c>
-      <c r="C20" s="4"/>
+      <c r="C20" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>20</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>21</v>
       </c>
-      <c r="C22" s="4"/>
+      <c r="C22" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>22</v>
       </c>
-      <c r="C23" s="4"/>
+      <c r="C23" s="4" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>23</v>
       </c>
-      <c r="C24" s="4"/>
+      <c r="C24" s="4" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="2">

</xml_diff>